<commit_message>
Added revised plotting code and plots.
</commit_message>
<xml_diff>
--- a/tests/test_results.xlsx
+++ b/tests/test_results.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/johnmsholar/Documents/Stanford/Courses/EE364B/LEigOpt/tests/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{490B411D-42A4-184D-A298-03AEA1487648}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E50AEA23-19CE-1B4C-9D9E-EA169046E14B}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="440" windowWidth="19200" windowHeight="21160" xr2:uid="{2EDEFD28-E3A6-4B4A-B9D2-916E04BFE6F6}"/>
+    <workbookView xWindow="0" yWindow="440" windowWidth="19200" windowHeight="20560" xr2:uid="{2EDEFD28-E3A6-4B4A-B9D2-916E04BFE6F6}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="11">
   <si>
     <t>b fixed</t>
   </si>
@@ -55,6 +55,9 @@
   </si>
   <si>
     <t xml:space="preserve">b </t>
+  </si>
+  <si>
+    <t>cvxopt-python</t>
   </si>
 </sst>
 </file>
@@ -406,10 +409,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{723479CE-F868-DA46-8DE9-AEC6DEF4243C}">
-  <dimension ref="A2:G26"/>
+  <dimension ref="A2:H26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -417,7 +420,7 @@
     <col min="4" max="4" width="15.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -439,8 +442,11 @@
       <c r="G2" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B3">
         <v>10</v>
       </c>
@@ -459,8 +465,11 @@
       <c r="G3" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H3">
+        <v>0.68500000000000005</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B4">
         <v>15</v>
       </c>
@@ -473,8 +482,11 @@
       <c r="F4">
         <v>1.984</v>
       </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H4">
+        <v>1.1850000000000001</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B5">
         <v>20</v>
       </c>
@@ -484,8 +496,11 @@
       <c r="F5">
         <v>3.42</v>
       </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H5">
+        <v>2.2170000000000001</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B6">
         <v>25</v>
       </c>
@@ -495,8 +510,11 @@
       <c r="F6">
         <v>5.7489999999999997</v>
       </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H6">
+        <v>2.778</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B7">
         <v>30</v>
       </c>
@@ -506,8 +524,11 @@
       <c r="F7">
         <v>8.8309999999999995</v>
       </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H7">
+        <v>4.5519999999999996</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B8">
         <v>35</v>
       </c>
@@ -517,8 +538,11 @@
       <c r="F8">
         <v>18.151</v>
       </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H8">
+        <v>6.42</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B9">
         <v>40</v>
       </c>
@@ -528,8 +552,11 @@
       <c r="F9">
         <v>30.433</v>
       </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H9">
+        <v>8.07</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B10">
         <v>45</v>
       </c>
@@ -539,8 +566,11 @@
       <c r="F10">
         <v>63.256</v>
       </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H10">
+        <v>10.365</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B11">
         <v>50</v>
       </c>
@@ -550,144 +580,192 @@
       <c r="F11">
         <v>93.908000000000001</v>
       </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H11">
+        <v>13.781000000000001</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B12">
+        <v>60</v>
+      </c>
+      <c r="C12">
+        <v>6.032</v>
+      </c>
+      <c r="H12">
+        <v>21.989000000000001</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B13">
         <v>75</v>
       </c>
-      <c r="C12">
-        <v>6.0330000000000004</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="B13">
+      <c r="C13">
+        <v>8.9689999999999994</v>
+      </c>
+      <c r="H13">
+        <v>45.43</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B14">
         <v>100</v>
       </c>
-      <c r="C13">
-        <v>10.032</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A15" t="s">
+      <c r="C14">
+        <v>17.699000000000002</v>
+      </c>
+      <c r="H14">
+        <v>112.952</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
         <v>8</v>
       </c>
-      <c r="B15" t="s">
+      <c r="B16" t="s">
         <v>9</v>
       </c>
-      <c r="C15" t="s">
+      <c r="C16" t="s">
         <v>2</v>
       </c>
-      <c r="D15" t="s">
+      <c r="D16" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="B16">
+      <c r="E16" t="s">
         <v>10</v>
       </c>
-      <c r="C16">
+    </row>
+    <row r="17" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B17">
+        <v>10</v>
+      </c>
+      <c r="C17">
         <v>0.51400000000000001</v>
       </c>
-      <c r="D16">
+      <c r="D17">
         <v>0.88400000000000001</v>
       </c>
-    </row>
-    <row r="17" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B17">
+      <c r="E17">
+        <v>0.77600000000000002</v>
+      </c>
+    </row>
+    <row r="18" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B18">
         <v>15</v>
       </c>
-      <c r="C17">
+      <c r="C18">
         <v>0.68899999999999995</v>
       </c>
-      <c r="D17">
+      <c r="D18">
         <v>2.1419999999999999</v>
       </c>
-    </row>
-    <row r="18" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B18">
+      <c r="E18">
+        <v>1.5069999999999999</v>
+      </c>
+    </row>
+    <row r="19" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B19">
         <v>20</v>
       </c>
-      <c r="C18">
+      <c r="C19">
         <v>0.90600000000000003</v>
       </c>
-      <c r="D18">
+      <c r="D19">
         <v>3.8820000000000001</v>
       </c>
-    </row>
-    <row r="19" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B19">
+      <c r="E19">
+        <v>2.5459999999999998</v>
+      </c>
+    </row>
+    <row r="20" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B20">
         <v>25</v>
       </c>
-      <c r="C19">
+      <c r="C20">
         <v>1.329</v>
       </c>
-      <c r="D19">
+      <c r="D20">
         <v>8.5570000000000004</v>
       </c>
-    </row>
-    <row r="20" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B20">
+      <c r="E20">
+        <v>3.6960000000000002</v>
+      </c>
+    </row>
+    <row r="21" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B21">
         <v>30</v>
       </c>
-      <c r="C20">
+      <c r="C21">
         <v>1.6910000000000001</v>
       </c>
-      <c r="D20">
+      <c r="D21">
         <v>11.057</v>
       </c>
-    </row>
-    <row r="21" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B21">
+      <c r="E21">
+        <v>5.2640000000000002</v>
+      </c>
+    </row>
+    <row r="22" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B22">
         <v>35</v>
       </c>
-      <c r="C21">
+      <c r="C22">
         <v>2.4710000000000001</v>
       </c>
-      <c r="D21">
+      <c r="D22">
         <v>18.957000000000001</v>
       </c>
-    </row>
-    <row r="22" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B22">
+      <c r="E22">
+        <v>7.8550000000000004</v>
+      </c>
+    </row>
+    <row r="23" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B23">
         <v>40</v>
       </c>
-      <c r="C22">
+      <c r="C23">
         <v>3.2080000000000002</v>
       </c>
-      <c r="D22">
+      <c r="D23">
         <v>29.727</v>
       </c>
-    </row>
-    <row r="23" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B23">
+      <c r="E23">
+        <v>10.154</v>
+      </c>
+    </row>
+    <row r="24" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B24">
         <v>45</v>
       </c>
-      <c r="C23">
+      <c r="C24">
         <v>4.2089999999999996</v>
       </c>
-      <c r="D23">
+      <c r="D24">
         <v>46.015999999999998</v>
       </c>
-    </row>
-    <row r="24" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B24">
+      <c r="E24">
+        <v>13.523</v>
+      </c>
+    </row>
+    <row r="25" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B25">
         <v>50</v>
       </c>
-      <c r="C24">
+      <c r="C25">
         <v>5.41</v>
       </c>
-      <c r="D24">
+      <c r="D25">
         <v>66.673000000000002</v>
       </c>
-    </row>
-    <row r="25" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B25">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="26" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="E25">
+        <v>18.93</v>
+      </c>
+    </row>
+    <row r="26" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B26">
-        <v>100</v>
+        <v>55</v>
+      </c>
+      <c r="C26">
+        <v>9.8680000000000003</v>
       </c>
     </row>
   </sheetData>

</xml_diff>